<commit_message>
menambahkan template_supply untuk import excel data supply
</commit_message>
<xml_diff>
--- a/UTS_POS/public/template_supply.xlsx
+++ b/UTS_POS/public/template_supply.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_DwiAhmadKhairy\UTS_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6F5DCF-11DD-4FFA-8027-338533775612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A22497-DABE-45F6-9FCA-D1713A23D43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15540" yWindow="1392" windowWidth="7500" windowHeight="11088" xr2:uid="{627A3C99-4863-4719-B148-124E320C6432}"/>
   </bookViews>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA2B5ED-CC7C-455E-A0C5-5EAF441DA12A}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,10 +440,65 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>2125000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1955000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2975000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3570000000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1360000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>1530000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>